<commit_message>
Update test report according to test17 change.
</commit_message>
<xml_diff>
--- a/documents/Team_Sprint4_Report.xlsx
+++ b/documents/Team_Sprint4_Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yn\Desktop\CS-555\week_11\Team_Ashish_Ning_Rohnit_Shivani_Report_Sprint4_End\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yn\Documents\ssw555group\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD80EF-EE63-468C-A204-48FDBDB112F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D0F345-3F8D-41AC-8D20-9A28453A414D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1091,12 +1091,6 @@
     <t>test17</t>
   </si>
   <si>
-    <t>us17_parent_ntmarry_children_check</t>
-  </si>
-  <si>
-    <t>9--22</t>
-  </si>
-  <si>
     <t>test39</t>
   </si>
   <si>
@@ -1140,6 +1134,12 @@
   </si>
   <si>
     <t>7--25</t>
+  </si>
+  <si>
+    <t>test_us17_parent_ntmarry_children_check</t>
+  </si>
+  <si>
+    <t>9--20</t>
   </si>
 </sst>
 </file>
@@ -28019,8 +28019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28134,10 +28134,10 @@
         <v>350</v>
       </c>
       <c r="P2" t="s">
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="Q2" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28179,13 +28179,13 @@
         <v>139140207208</v>
       </c>
       <c r="O4" t="s">
+        <v>360</v>
+      </c>
+      <c r="P4" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q4" t="s">
         <v>362</v>
-      </c>
-      <c r="P4" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28325,13 +28325,13 @@
         <v>342</v>
       </c>
       <c r="O10" t="s">
+        <v>363</v>
+      </c>
+      <c r="P10" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q10" t="s">
         <v>365</v>
-      </c>
-      <c r="P10" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28373,13 +28373,13 @@
         <v>338</v>
       </c>
       <c r="O12" t="s">
+        <v>351</v>
+      </c>
+      <c r="P12" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q12" t="s">
         <v>353</v>
-      </c>
-      <c r="P12" t="s">
-        <v>354</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28421,13 +28421,13 @@
         <v>334</v>
       </c>
       <c r="O14" t="s">
+        <v>354</v>
+      </c>
+      <c r="P14" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q14" t="s">
         <v>356</v>
-      </c>
-      <c r="P14" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28469,13 +28469,13 @@
         <v>336</v>
       </c>
       <c r="O16" t="s">
+        <v>357</v>
+      </c>
+      <c r="P16" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q16" t="s">
         <v>359</v>
-      </c>
-      <c r="P16" t="s">
-        <v>360</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update text output file and sprint 4 report accordingly.
</commit_message>
<xml_diff>
--- a/documents/Team_Sprint4_Report.xlsx
+++ b/documents/Team_Sprint4_Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yn\Documents\ssw555group\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yn\Desktop\CS-555\week_11\Team_Ashish_Ning_Rohnit_Shivani_Report_Sprint4_End\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D0F345-3F8D-41AC-8D20-9A28453A414D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A64EBBD-3B37-47C6-9F2E-30C8F1DDB072}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="369">
   <si>
     <t>Initials</t>
   </si>
@@ -1028,12 +1028,6 @@
     <t>us30_list_living_married</t>
   </si>
   <si>
-    <t>206--217</t>
-  </si>
-  <si>
-    <t>220--255</t>
-  </si>
-  <si>
     <t>us18_sibling_marriage</t>
   </si>
   <si>
@@ -1064,12 +1058,6 @@
     <t>We found one user story (unique ID) is more complicated than we thought and introduced changes to main class and multiple other user stories.</t>
   </si>
   <si>
-    <t>164--193</t>
-  </si>
-  <si>
-    <t>232--245</t>
-  </si>
-  <si>
     <t>us17_parent_ntmarry_children</t>
   </si>
   <si>
@@ -1140,6 +1128,21 @@
   </si>
   <si>
     <t>9--20</t>
+  </si>
+  <si>
+    <t>140--142, 208--210</t>
+  </si>
+  <si>
+    <t>232--248</t>
+  </si>
+  <si>
+    <t>228--263</t>
+  </si>
+  <si>
+    <t>215--225</t>
+  </si>
+  <si>
+    <t>166--195</t>
   </si>
 </sst>
 </file>
@@ -3786,7 +3789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E23" sqref="E23:E33"/>
     </sheetView>
   </sheetViews>
@@ -28020,7 +28023,7 @@
   <dimension ref="A1:Q1005"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28125,19 +28128,19 @@
         <v>243</v>
       </c>
       <c r="L2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="M2" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="O2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="P2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="Q2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28170,22 +28173,22 @@
         <v>43576</v>
       </c>
       <c r="K4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L4" t="s">
-        <v>340</v>
-      </c>
-      <c r="M4" s="33">
-        <v>139140207208</v>
+        <v>338</v>
+      </c>
+      <c r="M4" s="33" t="s">
+        <v>364</v>
       </c>
       <c r="O4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="P4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="Q4" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28221,19 +28224,19 @@
         <v>239</v>
       </c>
       <c r="L6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M6" t="s">
-        <v>331</v>
+        <v>366</v>
       </c>
       <c r="O6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="P6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="Q6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3">
@@ -28274,13 +28277,13 @@
         <v>329</v>
       </c>
       <c r="M8" t="s">
-        <v>330</v>
+        <v>367</v>
       </c>
       <c r="O8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="P8" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="Q8" t="s">
         <v>302</v>
@@ -28316,22 +28319,22 @@
         <v>43577</v>
       </c>
       <c r="K10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M10" t="s">
-        <v>342</v>
+        <v>368</v>
       </c>
       <c r="O10" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="P10" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="Q10" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28367,19 +28370,19 @@
         <v>238</v>
       </c>
       <c r="L12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="O12" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="P12" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="Q12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28415,19 +28418,19 @@
         <v>245</v>
       </c>
       <c r="L14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M14" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="O14" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="P14" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="Q14" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28463,19 +28466,19 @@
         <v>245</v>
       </c>
       <c r="L16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="P16" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="Q16" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -28494,7 +28497,7 @@
     </row>
     <row r="23" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="12" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>